<commit_message>
-- I live Gen Extr
</commit_message>
<xml_diff>
--- a/sample_data/out/POReport.xlsx
+++ b/sample_data/out/POReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\black-XL-ROSE\Documents\UiPath\Invoice_Document_Understanding\sample_data\out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEB28B5-8A51-45A6-88DC-F8123D72643D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56EB7A0-70A8-40FF-A5EB-BAF6728E140E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{3B97CAC1-8B63-4F31-B3FA-1ABEDD5F8BC9}"/>
+    <workbookView minimized="1" xWindow="975" yWindow="3720" windowWidth="14430" windowHeight="7725" activeTab="1" xr2:uid="{3B97CAC1-8B63-4F31-B3FA-1ABEDD5F8BC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Purchase Order Number</t>
   </si>
@@ -65,6 +65,48 @@
   </si>
   <si>
     <t>1748 S K Matseke Avenue, Munsieville, Krugersdorp, Johannesburg,</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Vendor Address</t>
+  </si>
+  <si>
+    <t>Shipping Name</t>
+  </si>
+  <si>
+    <t>Delivery by Date</t>
+  </si>
+  <si>
+    <t>Client Name</t>
+  </si>
+  <si>
+    <t>Client Address</t>
+  </si>
+  <si>
+    <t>#99674</t>
+  </si>
+  <si>
+    <t>31/08/2023</t>
+  </si>
+  <si>
+    <t>Leoba Connections (Pty) Ltd</t>
+  </si>
+  <si>
+    <t>103 Monale Street Munsieville</t>
+  </si>
+  <si>
+    <t>Lindiwe Mahlangu</t>
+  </si>
+  <si>
+    <t>1748 S K Matseke Avenue, Munsieville, Krugersdorp, Johannesburg, 1739</t>
+  </si>
+  <si>
+    <t>No deliveries will be accepted after 1500 without prior arrangement. 2. Site will not be held responsible for offloading any materials. 3. The rates quantities of this order are fixed. 4. Order discrepancies must be challenged before any deliveries start. 5. Motheo reserves the right to cancel or amend this order at any time.</t>
+  </si>
+  <si>
+    <t>Muhammed Saley</t>
   </si>
 </sst>
 </file>
@@ -100,9 +142,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,12 +528,83 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5980FDD3-2223-4674-ABFF-9DD311513D18}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2">
+        <v>398055.02</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45269</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>